<commit_message>
Add more results to Kmeans
</commit_message>
<xml_diff>
--- a/results/Spark_Kmeans_Data.xlsx
+++ b/results/Spark_Kmeans_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Time</t>
   </si>
@@ -53,6 +53,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -70,11 +71,12 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -122,12 +124,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -203,30 +209,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>K-means Running Time</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -237,7 +223,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$3</c:f>
+              <c:f>Sheet1!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -254,18 +240,34 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+              <c:f>Sheet1!$B$10:$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6000</c:v>
                 </c:pt>
               </c:strCache>
@@ -273,17 +275,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$D$3</c:f>
+              <c:f>Sheet1!$B$11:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>111.733</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>236.674</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1179</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2229</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3330</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4821</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -295,7 +306,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$4</c:f>
+              <c:f>Sheet1!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -312,18 +323,34 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+              <c:f>Sheet1!$B$10:$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6000</c:v>
                 </c:pt>
               </c:strCache>
@@ -331,17 +358,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$D$4</c:f>
+              <c:f>Sheet1!$B$12:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>112.542</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>243.528</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1316</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2453</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3510</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -353,7 +389,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5:$A$5</c:f>
+              <c:f>Sheet1!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -370,18 +406,34 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+              <c:f>Sheet1!$B$10:$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6000</c:v>
                 </c:pt>
               </c:strCache>
@@ -389,18 +441,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$D$5</c:f>
+              <c:f>Sheet1!$B$13:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>111.648</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>228.037</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>373.097</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>802</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1054</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1394</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2351</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2751</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -411,7 +472,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$6:$A$6</c:f>
+              <c:f>Sheet1!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -428,18 +489,34 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+              <c:f>Sheet1!$B$10:$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6000</c:v>
                 </c:pt>
               </c:strCache>
@@ -447,18 +524,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$D$6</c:f>
+              <c:f>Sheet1!$B$14:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>105.656</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>231.784</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>387.06</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1432</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1902</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -469,7 +555,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7:$A$7</c:f>
+              <c:f>Sheet1!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -486,18 +572,34 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+              <c:f>Sheet1!$B$10:$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6000</c:v>
                 </c:pt>
               </c:strCache>
@@ -505,29 +607,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$D$7</c:f>
+              <c:f>Sheet1!$B$15:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>101.347</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>209.822</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>373.029</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1730</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2362</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="41754899"/>
-        <c:axId val="82821286"/>
+        <c:overlap val="0"/>
+        <c:axId val="17767152"/>
+        <c:axId val="12178923"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41754899"/>
+        <c:axId val="17767152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -543,7 +655,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Cluster Size</a:t>
@@ -563,14 +675,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82821286"/>
+        <c:crossAx val="12178923"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82821286"/>
+        <c:axId val="12178923"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,10 +707,10 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Time (Seconds)</a:t>
+                  <a:t>Average Heap Utilization (MB)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -615,7 +727,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="41754899"/>
+        <c:crossAx val="17767152"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -650,30 +762,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>K-means Average Heap Utilization</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -684,7 +776,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11:$A$11</c:f>
+              <c:f>Sheet1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -701,18 +793,34 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$D$10</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+              <c:f>Sheet1!$B$2:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6000</c:v>
                 </c:pt>
               </c:strCache>
@@ -720,17 +828,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$D$11</c:f>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2229</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3839</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>61.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111.733</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>203.213</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>236.674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>350.961</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -742,7 +859,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$12:$A$12</c:f>
+              <c:f>Sheet1!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -759,18 +876,34 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$D$10</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+              <c:f>Sheet1!$B$2:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6000</c:v>
                 </c:pt>
               </c:strCache>
@@ -778,17 +911,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$D$12</c:f>
+              <c:f>Sheet1!$B$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2453</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4226</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>61.754</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112.542</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>192.201</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>243.528</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -800,7 +942,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$13:$A$13</c:f>
+              <c:f>Sheet1!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -817,18 +959,34 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$D$10</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+              <c:f>Sheet1!$B$2:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6000</c:v>
                 </c:pt>
               </c:strCache>
@@ -836,18 +994,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1054</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1801</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2751</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>56.745</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111.648</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>176.204</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>228.037</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>314.932</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>373.097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -858,7 +1025,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$14:$A$14</c:f>
+              <c:f>Sheet1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -875,18 +1042,34 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$D$10</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+              <c:f>Sheet1!$B$2:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6000</c:v>
                 </c:pt>
               </c:strCache>
@@ -894,18 +1077,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$D$14</c:f>
+              <c:f>Sheet1!$B$6:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1432</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2593</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3384</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>52.875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105.656</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>178.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>231.784</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>322.909</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>387.06</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -916,7 +1108,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15:$A$15</c:f>
+              <c:f>Sheet1!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -933,18 +1125,34 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$D$10</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+              <c:f>Sheet1!$B$2:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6000</c:v>
                 </c:pt>
               </c:strCache>
@@ -952,29 +1160,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$D$15</c:f>
+              <c:f>Sheet1!$B$7:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1259</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2362</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3159</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50.894</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101.347</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160.024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>209.822</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>298.995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>373.029</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="87890976"/>
-        <c:axId val="87117100"/>
+        <c:overlap val="0"/>
+        <c:axId val="94903423"/>
+        <c:axId val="85779787"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87890976"/>
+        <c:axId val="94903423"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +1208,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Cluster Size</a:t>
@@ -1010,14 +1228,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="87117100"/>
+        <c:crossAx val="85779787"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87117100"/>
+        <c:axId val="85779787"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1042,10 +1260,10 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Average Heap Utilization (MB)</a:t>
+                  <a:t>Time (Seconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1062,7 +1280,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="87890976"/>
+        <c:crossAx val="94903423"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1102,15 +1320,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>217080</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>284400</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>622440</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1118,8 +1336,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="217080" y="2744280"/>
-        <a:ext cx="5762520" cy="3241800"/>
+        <a:off x="244080" y="2735280"/>
+        <a:ext cx="7738560" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1131,16 +1349,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>677160</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>56880</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>122400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>609480</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>759600</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1148,8 +1366,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6372360" y="2627280"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="8249400" y="2560680"/>
+        <a:ext cx="8195040" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1167,10 +1385,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1187,12 +1405,21 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>4000</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="F2" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>6000</v>
       </c>
     </row>
@@ -1201,12 +1428,21 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="n">
+        <v>61.625</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>111.733</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
+        <v>203.213</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>236.674</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="0" t="n">
+        <v>350.961</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1215,12 +1451,21 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
+        <v>61.754</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>112.542</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
+        <v>192.201</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>243.528</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="F4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1228,13 +1473,22 @@
       <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="0" t="n">
+        <v>56.745</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>111.648</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="D5" s="0" t="n">
+        <v>176.204</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>228.037</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="F5" s="0" t="n">
+        <v>314.932</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>373.097</v>
       </c>
     </row>
@@ -1242,13 +1496,22 @@
       <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
+        <v>52.875</v>
+      </c>
+      <c r="C6" s="0" t="n">
         <v>105.656</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="D6" s="0" t="n">
+        <v>178.62</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>231.784</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="F6" s="0" t="n">
+        <v>322.909</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>387.06</v>
       </c>
     </row>
@@ -1257,12 +1520,21 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
+        <v>50.894</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>101.347</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="D7" s="0" t="n">
+        <v>160.024</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>209.822</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="F7" s="0" t="n">
+        <v>298.995</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>373.029</v>
       </c>
     </row>
@@ -1273,12 +1545,21 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="D10" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E10" s="0" t="n">
         <v>4000</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="F10" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>6000</v>
       </c>
     </row>
@@ -1287,12 +1568,21 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="n">
+        <v>1179</v>
+      </c>
+      <c r="C11" s="0" t="n">
         <v>2229</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="D11" s="0" t="n">
+        <v>3330</v>
+      </c>
+      <c r="E11" s="0" t="n">
         <v>3839</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="F11" s="0" t="n">
+        <v>4821</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1300,13 +1590,22 @@
       <c r="A12" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="0" t="n">
+        <v>1316</v>
+      </c>
+      <c r="C12" s="1" t="n">
         <v>2453</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="D12" s="0" t="n">
+        <v>3510</v>
+      </c>
+      <c r="E12" s="0" t="n">
         <v>4226</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="F12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1314,13 +1613,22 @@
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="0" t="n">
+        <v>802</v>
+      </c>
+      <c r="C13" s="1" t="n">
         <v>1054</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="D13" s="0" t="n">
+        <v>1394</v>
+      </c>
+      <c r="E13" s="0" t="n">
         <v>1801</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="F13" s="0" t="n">
+        <v>2351</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>2751</v>
       </c>
     </row>
@@ -1328,13 +1636,22 @@
       <c r="A14" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="0" t="n">
+        <v>952</v>
+      </c>
+      <c r="C14" s="1" t="n">
         <v>1432</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="D14" s="0" t="n">
+        <v>1902</v>
+      </c>
+      <c r="E14" s="0" t="n">
         <v>2593</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="F14" s="0" t="n">
+        <v>2974</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>3384</v>
       </c>
     </row>
@@ -1343,12 +1660,21 @@
         <v>6</v>
       </c>
       <c r="B15" s="0" t="n">
+        <v>995</v>
+      </c>
+      <c r="C15" s="0" t="n">
         <v>1259</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="D15" s="0" t="n">
+        <v>1730</v>
+      </c>
+      <c r="E15" s="0" t="n">
         <v>2362</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="F15" s="0" t="n">
+        <v>2900</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>3159</v>
       </c>
     </row>

</xml_diff>